<commit_message>
Java with Selenium Project
</commit_message>
<xml_diff>
--- a/Output/MarketData.xlsx
+++ b/Output/MarketData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>Index</t>
   </si>
@@ -29,178 +29,175 @@
     <t>BSE Cons Durable</t>
   </si>
   <si>
-    <t>37944.83</t>
-  </si>
-  <si>
-    <t>-168.28</t>
-  </si>
-  <si>
-    <t>-0.44</t>
+    <t>37527.22</t>
+  </si>
+  <si>
+    <t>355.65</t>
+  </si>
+  <si>
+    <t>0.96</t>
   </si>
   <si>
     <t>BSE FMCG</t>
   </si>
   <si>
-    <t>16520.89</t>
-  </si>
-  <si>
-    <t>84.56</t>
-  </si>
-  <si>
-    <t>0.51</t>
+    <t>16130.91</t>
+  </si>
+  <si>
+    <t>99.64</t>
+  </si>
+  <si>
+    <t>0.62</t>
   </si>
   <si>
     <t>BSE Healthcare</t>
   </si>
   <si>
-    <t>21695.88</t>
-  </si>
-  <si>
-    <t>-82.68</t>
-  </si>
-  <si>
-    <t>-0.38</t>
+    <t>21663.67</t>
+  </si>
+  <si>
+    <t>133.06</t>
   </si>
   <si>
     <t>BSE Metals</t>
   </si>
   <si>
-    <t>19559.76</t>
-  </si>
-  <si>
-    <t>-84.49</t>
-  </si>
-  <si>
-    <t>-0.43</t>
+    <t>19047.76</t>
+  </si>
+  <si>
+    <t>-527.96</t>
+  </si>
+  <si>
+    <t>-2.70</t>
   </si>
   <si>
     <t>BSE Oil &amp; Gas</t>
   </si>
   <si>
-    <t>17772.01</t>
-  </si>
-  <si>
-    <t>138.55</t>
-  </si>
-  <si>
-    <t>0.79</t>
+    <t>17635.55</t>
+  </si>
+  <si>
+    <t>253.22</t>
+  </si>
+  <si>
+    <t>1.46</t>
   </si>
   <si>
     <t>BSE Teck</t>
   </si>
   <si>
-    <t>13547.13</t>
-  </si>
-  <si>
-    <t>-47.85</t>
-  </si>
-  <si>
-    <t>-0.35</t>
+    <t>12925.67</t>
+  </si>
+  <si>
+    <t>-42.36</t>
+  </si>
+  <si>
+    <t>-0.33</t>
   </si>
   <si>
     <t>Nifty PSE</t>
   </si>
   <si>
-    <t>4606.45</t>
-  </si>
-  <si>
-    <t>43.10</t>
-  </si>
-  <si>
-    <t>0.94</t>
+    <t>4564.55</t>
+  </si>
+  <si>
+    <t>33.45</t>
+  </si>
+  <si>
+    <t>0.74</t>
   </si>
   <si>
     <t>Nifty 50</t>
   </si>
   <si>
-    <t>17754.40</t>
-  </si>
-  <si>
-    <t>42.90</t>
-  </si>
-  <si>
-    <t>0.24</t>
+    <t>16986.20</t>
+  </si>
+  <si>
+    <t>14.00</t>
+  </si>
+  <si>
+    <t>0.08</t>
   </si>
   <si>
     <t>BSE Sensex</t>
   </si>
   <si>
-    <t>60348.09</t>
-  </si>
-  <si>
-    <t>123.63</t>
-  </si>
-  <si>
-    <t>0.21</t>
+    <t>57618.96</t>
+  </si>
+  <si>
+    <t>63.06</t>
+  </si>
+  <si>
+    <t>0.11</t>
   </si>
   <si>
     <t>Nifty Bank</t>
   </si>
   <si>
-    <t>41577.10</t>
-  </si>
-  <si>
-    <t>226.70</t>
-  </si>
-  <si>
-    <t>0.55</t>
+    <t>39063.20</t>
+  </si>
+  <si>
+    <t>11.70</t>
+  </si>
+  <si>
+    <t>0.03</t>
   </si>
   <si>
     <t>Nifty IT</t>
   </si>
   <si>
-    <t>30065.80</t>
-  </si>
-  <si>
-    <t>-113.95</t>
+    <t>28557.80</t>
+  </si>
+  <si>
+    <t>-158.70</t>
+  </si>
+  <si>
+    <t>-0.55</t>
   </si>
   <si>
     <t>BSE SmallCap</t>
   </si>
   <si>
-    <t>28173.46</t>
-  </si>
-  <si>
-    <t>77.43</t>
-  </si>
-  <si>
-    <t>0.28</t>
+    <t>27020.77</t>
+  </si>
+  <si>
+    <t>-148.39</t>
   </si>
   <si>
     <t>BSE MidCap</t>
   </si>
   <si>
-    <t>24925.18</t>
-  </si>
-  <si>
-    <t>151.63</t>
-  </si>
-  <si>
-    <t>0.61</t>
+    <t>24069.54</t>
+  </si>
+  <si>
+    <t>16.34</t>
+  </si>
+  <si>
+    <t>0.07</t>
   </si>
   <si>
     <t>Nifty Auto</t>
   </si>
   <si>
-    <t>13019.50</t>
-  </si>
-  <si>
-    <t>110.00</t>
-  </si>
-  <si>
-    <t>0.85</t>
+    <t>12319.30</t>
+  </si>
+  <si>
+    <t>37.30</t>
+  </si>
+  <si>
+    <t>0.30</t>
   </si>
   <si>
     <t>BSE Cap Goods</t>
   </si>
   <si>
-    <t>34813.43</t>
-  </si>
-  <si>
-    <t>423.64</t>
-  </si>
-  <si>
-    <t>1.23</t>
+    <t>34235.34</t>
+  </si>
+  <si>
+    <t>-123.03</t>
+  </si>
+  <si>
+    <t>-0.36</t>
   </si>
 </sst>
 </file>
@@ -304,119 +301,119 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>34</v>
-      </c>
-      <c r="D9" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>38</v>
-      </c>
-      <c r="D10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>42</v>
-      </c>
-      <c r="D11" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
         <v>44</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>46</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="13">
@@ -430,49 +427,49 @@
         <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
         <v>51</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>52</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>53</v>
-      </c>
-      <c r="D14" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
         <v>55</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>56</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>57</v>
-      </c>
-      <c r="D15" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
         <v>59</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>60</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>61</v>
-      </c>
-      <c r="D16" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>